<commit_message>
case gender and published in objects corrected. New input xl for ccdc
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Canine_MFST_SamplePatho-TCellLymphoma.xlsx
+++ b/InputFiles/TC02_Canine_MFST_SamplePatho-TCellLymphoma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\June\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\July\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070024B4-A2FB-40BA-BFED-16D4B3B39237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED711376-AC78-4F99-BE45-AE1B443DCA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -67,28 +67,6 @@
   </si>
   <si>
     <t>StudyFilesTab</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-MATCH (c)&lt;--(diag:diagnosis) 
- MATCH (samp:sample)--&gt;(c)
- WHERE samp.specific_sample_pathology IN  ['T Cell Lymphoma']
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
-RETURN  
-       coalesce(c.case_id, '') AS `Case ID`,
-       coalesce(s.clinical_study_designation, '') AS `Study Code`,
-       coalesce(s.clinical_study_type, '') AS  `Study Type`,
-       coalesce(demo.breed, '') AS Breed ,
-       coalesce(diag.disease_term, '') AS Diagnosis ,
-       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
-       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
-       coalesce(demo.sex, '') AS Sex,
-       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-       coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
-       coalesce(diag.best_response, '') AS `Response to Treatment`,
-       coalesce(co.cohort_description, '') AS `Cohort`
-Order by c.case_id LIMIT 100</t>
   </si>
   <si>
     <t xml:space="preserve"> 
@@ -185,45 +163,70 @@
   coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
   <si>
-    <t>MATCH (samp:sample)
-WHERE samp.specific_sample_pathology IN ['T Cell Lymphoma']
-MATCH (samp)--&gt;(c:case)--&gt;(s:study)
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (c)&lt;--(diag:diagnosis) 
+ MATCH (samp:sample)--&gt;(c)
+ WHERE samp.specific_sample_pathology IN  ['T Cell Lymphoma']
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage Of Disease`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+       coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`
+Order by c.case_id LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (samp:sample)--&gt;(c:case)
+WHERE 
+  samp.specific_sample_pathology IN  ['T Cell Lymphoma']
+WITH c
 MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (f)--&gt;(samp:sample)
 OPTIONAL MATCH (f)--&gt;(parent)
+OPTIONAL MATCH (c)--&gt;(s:study)
 OPTIONAL MATCH (c)--&gt;(cv:canine_individual)
+WITH 
+  DISTINCT f, samp, c, s, cv, parent,
+  ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+  toInteger(floor(log(f.file_size)/log(1024))) as i,
+  2 as precision
+WITH 
+  samp, c, s, f, cv, parent,
+  f.file_size /(1024^i) AS value,
+  10^precision AS factor,
+  units[i] as unit
 WITH
-	DISTINCT f, samp, c, s, parent, cv,
-  	['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-	toInteger(floor(log(f.file_size)/log(1024))) as i,
-	2 as precision
- WITH
-  	samp, c, s, f, parent, cv,
-    f.file_size /(1024^i) AS value,
-    10^precision AS factor,
-    units[i] as unit
-WITH
-    samp, c, s, f, unit, parent, cv,
-    round(factor * value)/factor AS size
+  samp, c, s, f, cv, parent, unit,
+  round(factor * value)/factor AS size
 RETURN
-	coalesce(f.file_name, '') AS `File Name`,
-	coalesce(f.file_format, '') AS `Format`,
-	coalesce(f.file_type, '') AS `File Type`,
-	CASE size % 1
-	  WHEN 0
-	  THEN apoc.convert.toInteger(size)+' ' +unit
-	  ELSE size+' ' +unit
-	END AS Size,
-	head(labels(parent)) AS `Association`,
-	coalesce(f.file_description,'') AS `Description`,
-	coalesce(samp.sample_id, '') AS `Sample ID`,
-	coalesce(c.case_id,'') as `Case ID`,
-	coalesce(cv.canine_individual_id,'') AS `Canine ID`,
-	CASE
-	  WHEN s.clinical_study_designation IS NULL
-	  THEN parent.clinical_study_designation
-	  ELSE s.clinical_study_designation
-	END AS `Study Code`
-ORDER BY `File Name`
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_format, '') AS `Format`,
+  coalesce(f.file_type, '') AS `File Type`,
+  CASE size % 1 
+      WHEN 0 
+      THEN apoc.convert.toInteger(size)+' ' +unit 
+      ELSE size+' ' +unit 
+  END AS Size,
+  head(labels(parent)) AS `Association`,
+  coalesce(f.file_description,'') AS `Description`,
+  coalesce(samp.sample_id, '') AS `Sample ID`,
+  coalesce(c.case_id,'') as `Case ID`,
+  coalesce(cv.canine_individual_id,'') AS `Canine ID`,
+  CASE 
+      WHEN s.clinical_study_designation IS NULL
+      THEN parent.clinical_study_designation
+      ELSE s.clinical_study_designation 
+  END AS `Study Code`
+ORDER BY `File Name` 
 LIMIT 100</t>
   </si>
 </sst>
@@ -596,20 +599,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.42578125" customWidth="1"/>
-    <col min="3" max="4" width="75.7109375" customWidth="1"/>
-    <col min="5" max="5" width="70.28515625" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.453125" customWidth="1"/>
+    <col min="3" max="4" width="75.7265625" customWidth="1"/>
+    <col min="5" max="5" width="70.26953125" customWidth="1"/>
+    <col min="6" max="6" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -629,15 +632,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -649,15 +652,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>17</v>
@@ -669,15 +672,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
@@ -689,15 +692,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>

</xml_diff>